<commit_message>
change JourNo in Vouchers and journal entry
</commit_message>
<xml_diff>
--- a/FileProject/النماذج.xlsx
+++ b/FileProject/النماذج.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProject\OilStationW\FileProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF6901-E91B-4100-85CA-69565660DE61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA950C8-453A-4A78-B4A3-11AA3EE5E245}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20640" windowHeight="11310" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="101">
   <si>
     <t>الحقل</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>حساب محطة العبور</t>
+  </si>
+  <si>
+    <t>حسابات الادارة</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1043,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1141,7 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>